<commit_message>
Add support for cell preview.
</commit_message>
<xml_diff>
--- a/tests/xlsx/rich-text.xlsx
+++ b/tests/xlsx/rich-text.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10609"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD243AD7-9C7E-D248-A4EE-4668576491B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="22260" windowHeight="12640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,15 +19,197 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">aaa        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>a</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">a </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">aaa aaa </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>aa</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>b</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>bbbbbb</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>AB</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="14"/>
+        <color rgb="FFFFFF00"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t>C</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FFFFFF00"/>
+        <rFont val="Helvetica"/>
+        <family val="2"/>
+      </rPr>
+      <t>DEFG</t>
+    </r>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B0F0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF00B0F0"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FFFFFF00"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="14"/>
+      <color rgb="FFFFFF00"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -49,8 +232,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,81 +516,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="inlineStr">
-        <is>
-          <r>
-            <rPr>
-              <b/>
-              <sz val="11"/>
-              <color theme="1"/>
-              <name val="等线"/>
-              <family val="3"/>
-              <charset val="134"/>
-              <scheme val="minor"/>
-            </rPr>
-            <t>aaa</t>
-          </r>
-          <r>
-            <rPr>
-              <sz val="11"/>
-              <color theme="1"/>
-              <name val="等线"/>
-              <family val="2"/>
-              <scheme val="minor"/>
-            </rPr>
-            <t>a</t>
-          </r>
-          <r>
-            <rPr>
-              <i/>
-              <sz val="11"/>
-              <color theme="1"/>
-              <name val="等线"/>
-              <family val="3"/>
-              <charset val="134"/>
-              <scheme val="minor"/>
-            </rPr>
-            <t>a</t>
-          </r>
-          <r>
-            <rPr>
-              <i/>
-              <sz val="11"/>
-              <color rgb="FFFF0000"/>
-              <name val="等线"/>
-              <family val="3"/>
-              <charset val="134"/>
-              <scheme val="minor"/>
-            </rPr>
-            <t>aaaaaa</t>
-          </r>
-          <r>
-            <rPr>
-              <sz val="11"/>
-              <color rgb="FFFF0000"/>
-              <name val="等线"/>
-              <family val="3"/>
-              <charset val="134"/>
-              <scheme val="minor"/>
-            </rPr>
-            <t>aa</t>
-          </r>
-        </is>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>